<commit_message>
Admin Info Details updated
Admin Info Details updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/Anodiam-Info/Anodiam-Info-Details.xlsx
+++ b/Offline/BusinessManagement/Information/Anodiam-Info/Anodiam-Info-Details.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Student-Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Anodiam-Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2F332E-A1BB-4E19-9B37-59ECB1CC9A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7E2C1E-57AB-4379-A964-47BA0422106D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Attendance-Details" sheetId="1" r:id="rId1"/>
+    <sheet name="Student-Attendance-Details" sheetId="1" r:id="rId1"/>
     <sheet name="Faculty-Pay-Details" sheetId="2" r:id="rId2"/>
+    <sheet name="APP-QC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Student Name</t>
   </si>
@@ -98,6 +99,51 @@
   </si>
   <si>
     <t xml:space="preserve">Mrs.Sanjukta ghosh </t>
+  </si>
+  <si>
+    <t>Fees Amt</t>
+  </si>
+  <si>
+    <t>Payment Date</t>
+  </si>
+  <si>
+    <t>Payment For Sep-2023</t>
+  </si>
+  <si>
+    <t>App Name</t>
+  </si>
+  <si>
+    <t>Ticket No</t>
+  </si>
+  <si>
+    <t>Issuer Name</t>
+  </si>
+  <si>
+    <t>Ticket Details</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Ticket Date</t>
+  </si>
+  <si>
+    <t>ClassPlus</t>
+  </si>
+  <si>
+    <t>Urgent Show Stopper Bug. No Access for Admins</t>
+  </si>
+  <si>
+    <t>Anirban Chakraborty</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Closing Date</t>
   </si>
 </sst>
 </file>
@@ -152,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -188,11 +234,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -214,7 +297,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +635,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>7</v>
@@ -730,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>7</v>
@@ -1077,36 +1179,523 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F539B8-F119-4E5F-8A5D-344EE98BF31C}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="14">
+        <v>45170</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="11">
+        <v>4000</v>
+      </c>
+      <c r="E8" s="12">
+        <v>45204</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5914FF4-7A80-408F-9750-849ED1020382}">
+  <dimension ref="A1:I33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1282691</v>
+      </c>
+      <c r="D2" s="20">
+        <v>45205</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Anodiam Info Details updated
Anodiam Info Details updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/Anodiam-Info/Anodiam-Info-Details.xlsx
+++ b/Offline/BusinessManagement/Information/Anodiam-Info/Anodiam-Info-Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Anodiam-Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C83896C-A4A9-4F50-BBBD-4D14EF31BD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D29BE16-91FB-42E2-887C-C39371349241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,9 +150,6 @@
     <t>Course</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>HOD Approval(Y/N)</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>HOD Name</t>
+  </si>
+  <si>
+    <t>Chapter Details/Link</t>
   </si>
 </sst>
 </file>
@@ -370,21 +370,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -403,6 +388,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1286,30 +1286,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
@@ -1792,13 +1792,14 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -1807,89 +1808,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="G1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="H1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="I1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="28" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
-        <v>1</v>
-      </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21">
-        <v>2</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-    </row>
-    <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21">
-        <v>3</v>
-      </c>
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21">
-        <v>4</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>